<commit_message>
Glyph plotting for CBBP substitute for Parallelplot
</commit_message>
<xml_diff>
--- a/inventory-biocytin-raw-37-layerdepth.xlsx
+++ b/inventory-biocytin-raw-37-layerdepth.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="899"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="733"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="13" r:id="rId1"/>
@@ -1319,11 +1319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="260687584"/>
-        <c:axId val="260691936"/>
+        <c:axId val="-1117660336"/>
+        <c:axId val="-1117650000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="260687584"/>
+        <c:axId val="-1117660336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,12 +1380,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260691936"/>
+        <c:crossAx val="-1117650000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="260691936"/>
+        <c:axId val="-1117650000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,7 +1442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260687584"/>
+        <c:crossAx val="-1117660336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1531,7 +1531,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1806,11 +1805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="295182560"/>
-        <c:axId val="295183648"/>
+        <c:axId val="-1117657616"/>
+        <c:axId val="-1117665232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="295182560"/>
+        <c:axId val="-1117657616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,12 +1866,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295183648"/>
+        <c:crossAx val="-1117665232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="295183648"/>
+        <c:axId val="-1117665232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1929,7 +1928,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295182560"/>
+        <c:crossAx val="-1117657616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3447,7 +3446,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,6 +3880,10 @@
       <c r="AI3" s="7">
         <v>649.9139993601832</v>
       </c>
+      <c r="AJ3" s="7">
+        <f>AH3/AI3</f>
+        <v>0.90781241915212418</v>
+      </c>
       <c r="AK3" s="7">
         <f>SUM(AP3:AS3)</f>
         <v>14</v>
@@ -4069,8 +4072,12 @@
       <c r="AI4" s="7">
         <v>991.98325620000003</v>
       </c>
+      <c r="AJ4" s="7">
+        <f t="shared" ref="AJ4:AJ33" si="7">AH4/AI4</f>
+        <v>0.87400668769473533</v>
+      </c>
       <c r="AK4" s="7">
-        <f t="shared" ref="AK4:AK27" si="7">SUM(AP4:AS4)</f>
+        <f t="shared" ref="AK4:AK27" si="8">SUM(AP4:AS4)</f>
         <v>8</v>
       </c>
       <c r="AL4" s="7">
@@ -4090,19 +4097,19 @@
         <v>0.25</v>
       </c>
       <c r="AP4" s="6">
-        <f t="shared" ref="AP4:AP33" si="8">COUNTIF($AT4:$BM4,"&gt;=0")-COUNTIF($AT4:$BM4,"&gt;45")</f>
+        <f t="shared" ref="AP4:AP33" si="9">COUNTIF($AT4:$BM4,"&gt;=0")-COUNTIF($AT4:$BM4,"&gt;45")</f>
         <v>0</v>
       </c>
       <c r="AQ4" s="6">
-        <f t="shared" ref="AQ4:AQ33" si="9">COUNTIF($AT4:$BM4,"&gt;=45")-COUNTIF($AT4:$BM4,"&gt;90")</f>
+        <f t="shared" ref="AQ4:AQ33" si="10">COUNTIF($AT4:$BM4,"&gt;=45")-COUNTIF($AT4:$BM4,"&gt;90")</f>
         <v>2</v>
       </c>
       <c r="AR4" s="6">
-        <f t="shared" ref="AR4:AR33" si="10">COUNTIF($AT4:$BM4,"&gt;=90")-COUNTIF($AT4:$BM4,"&gt;135")</f>
+        <f t="shared" ref="AR4:AR33" si="11">COUNTIF($AT4:$BM4,"&gt;=90")-COUNTIF($AT4:$BM4,"&gt;135")</f>
         <v>4</v>
       </c>
       <c r="AS4" s="6">
-        <f t="shared" ref="AS4:AS33" si="11">COUNTIF($AT4:$BM4,"&gt;=135")-COUNTIF($AT4:$BM4,"&gt;180")</f>
+        <f t="shared" ref="AS4:AS33" si="12">COUNTIF($AT4:$BM4,"&gt;=135")-COUNTIF($AT4:$BM4,"&gt;180")</f>
         <v>2</v>
       </c>
       <c r="AT4" s="19">
@@ -4238,14 +4245,18 @@
         <v>0.58936484490398822</v>
       </c>
       <c r="AH5" s="7">
-        <f t="shared" ref="AH5:AH28" si="12">AE5+AF5</f>
+        <f t="shared" ref="AH5:AH28" si="13">AE5+AF5</f>
         <v>677</v>
       </c>
       <c r="AI5" s="7">
         <v>669.73832810924898</v>
       </c>
+      <c r="AJ5" s="7">
+        <f t="shared" si="7"/>
+        <v>1.0108425508679659</v>
+      </c>
       <c r="AK5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AL5" s="7">
@@ -4265,19 +4276,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AP5" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ5" s="6">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="AR5" s="6">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
+      <c r="AR5" s="6">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
       <c r="AS5" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT5" s="19">
@@ -4407,14 +4418,18 @@
         <v>9.166666666666666E-2</v>
       </c>
       <c r="AH6" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>840</v>
       </c>
       <c r="AI6" s="7">
         <v>1017.5093052750927</v>
       </c>
+      <c r="AJ6" s="7">
+        <f t="shared" si="7"/>
+        <v>0.82554527574850878</v>
+      </c>
       <c r="AK6" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="AL6" s="7">
@@ -4434,19 +4449,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AP6" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AQ6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AR6" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS6" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT6" s="19">
@@ -4581,14 +4596,18 @@
         <v>0.536036036036036</v>
       </c>
       <c r="AH7" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>888</v>
       </c>
       <c r="AI7" s="7">
         <v>945.94926434252636</v>
       </c>
+      <c r="AJ7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.93873956402640313</v>
+      </c>
       <c r="AK7" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="AL7" s="7">
@@ -4608,19 +4627,19 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="AP7" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ7" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AR7" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS7" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="AT7" s="19">
@@ -4760,8 +4779,12 @@
       <c r="AI8" s="7">
         <v>1132.7984365277587</v>
       </c>
+      <c r="AJ8" s="7">
+        <f t="shared" si="7"/>
+        <v>1.084041044198518</v>
+      </c>
       <c r="AK8" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AL8" s="7">
@@ -4781,19 +4804,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AP8" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ8" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AR8" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS8" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT8" s="19">
@@ -4929,8 +4952,12 @@
       <c r="AI9" s="7">
         <v>1132.7984365277587</v>
       </c>
+      <c r="AJ9" s="7">
+        <f t="shared" si="7"/>
+        <v>0.88806619744601711</v>
+      </c>
       <c r="AK9" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL9" s="7">
@@ -4950,19 +4977,19 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="AP9" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="6">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AQ9" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="AR9" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="AS9" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT9" s="19">
@@ -5105,8 +5132,12 @@
       <c r="AI10" s="7">
         <v>1068.1788927303846</v>
       </c>
+      <c r="AJ10" s="7">
+        <f t="shared" si="7"/>
+        <v>0.93242808557479795</v>
+      </c>
       <c r="AK10" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL10" s="7">
@@ -5126,19 +5157,19 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="AP10" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ10" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AR10" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AS10" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="AT10" s="19">
@@ -5273,8 +5304,12 @@
       <c r="AI11" s="7">
         <v>1068.1788927303846</v>
       </c>
+      <c r="AJ11" s="7">
+        <f t="shared" si="7"/>
+        <v>0.96519413275865129</v>
+      </c>
       <c r="AK11" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AL11" s="7">
@@ -5294,19 +5329,19 @@
         <v>0.6</v>
       </c>
       <c r="AP11" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ11" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AR11" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AS11" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT11" s="19">
@@ -5439,8 +5474,12 @@
       <c r="AI12" s="7">
         <v>1180.2462890625</v>
       </c>
+      <c r="AJ12" s="7">
+        <f t="shared" si="7"/>
+        <v>0.8769356104666316</v>
+      </c>
       <c r="AK12" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="AL12" s="7">
@@ -5460,19 +5499,19 @@
         <v>0.25</v>
       </c>
       <c r="AP12" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ12" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AR12" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="AS12" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT12" s="19">
@@ -5621,8 +5660,12 @@
       <c r="AI13" s="7">
         <v>851.99810165014026</v>
       </c>
+      <c r="AJ13" s="7">
+        <f t="shared" si="7"/>
+        <v>1.117373381649768</v>
+      </c>
       <c r="AK13" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="AL13" s="7">
@@ -5642,19 +5685,19 @@
         <v>0.1</v>
       </c>
       <c r="AP13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ13" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="AR13" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="AS13" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="AT13" s="19">
@@ -5797,8 +5840,12 @@
       <c r="AI14" s="7">
         <v>828.83616819220072</v>
       </c>
+      <c r="AJ14" s="7">
+        <f t="shared" si="7"/>
+        <v>0.79871031864343944</v>
+      </c>
       <c r="AK14" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AL14" s="7">
@@ -5818,19 +5865,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AP14" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ14" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AR14" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS14" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT14" s="19">
@@ -5961,8 +6008,12 @@
       <c r="AI15" s="7">
         <v>975.75031895791335</v>
       </c>
+      <c r="AJ15" s="7">
+        <f t="shared" si="7"/>
+        <v>1.0023055908856779</v>
+      </c>
       <c r="AK15" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="AL15" s="7">
@@ -5982,19 +6033,19 @@
         <v>0.22222222222222221</v>
       </c>
       <c r="AP15" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AR15" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="AS15" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT15" s="19">
@@ -6136,8 +6187,12 @@
       <c r="AI16" s="7">
         <v>1111.3017013549804</v>
       </c>
+      <c r="AJ16" s="7">
+        <f t="shared" si="7"/>
+        <v>0.88274858105939458</v>
+      </c>
       <c r="AK16" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL16" s="7">
@@ -6157,19 +6212,19 @@
         <v>0.42857142857142855</v>
       </c>
       <c r="AP16" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ16" s="6">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="AR16" s="6">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
+      <c r="AR16" s="6">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
       <c r="AS16" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT16" s="19">
@@ -6300,14 +6355,18 @@
         <v>0.6741573033707865</v>
       </c>
       <c r="AH17" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>712</v>
       </c>
       <c r="AI17" s="7">
         <v>759.49294339693506</v>
       </c>
+      <c r="AJ17" s="7">
+        <f t="shared" si="7"/>
+        <v>0.93746756463000636</v>
+      </c>
       <c r="AK17" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="AL17" s="7">
@@ -6327,19 +6386,19 @@
         <v>0.27272727272727271</v>
       </c>
       <c r="AP17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ17" s="6">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="AR17" s="6">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
+      <c r="AR17" s="6">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
       <c r="AS17" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT17" s="19">
@@ -6480,14 +6539,18 @@
         <v>0.38687150837988826</v>
       </c>
       <c r="AH18" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>716</v>
       </c>
       <c r="AI18" s="7">
         <v>759.49294339693506</v>
       </c>
+      <c r="AJ18" s="7">
+        <f t="shared" si="7"/>
+        <v>0.94273423634141096</v>
+      </c>
       <c r="AK18" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="AL18" s="7">
@@ -6507,19 +6570,19 @@
         <v>0.1875</v>
       </c>
       <c r="AP18" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ18" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="AR18" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="AS18" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT18" s="19">
@@ -6680,8 +6743,12 @@
       <c r="AI19" s="7">
         <v>700.88126220703123</v>
       </c>
+      <c r="AJ19" s="7">
+        <f t="shared" si="7"/>
+        <v>1.000169412137792</v>
+      </c>
       <c r="AK19" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="AL19" s="7">
@@ -6701,19 +6768,19 @@
         <v>0.375</v>
       </c>
       <c r="AP19" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AQ19" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AR19" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS19" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT19" s="19">
@@ -6851,8 +6918,12 @@
       <c r="AI20" s="7">
         <v>852.2952910632622</v>
       </c>
+      <c r="AJ20" s="7">
+        <f t="shared" si="7"/>
+        <v>0.92925539810498992</v>
+      </c>
       <c r="AK20" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="AL20" s="7">
@@ -6872,19 +6943,19 @@
         <v>0.2</v>
       </c>
       <c r="AP20" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ20" s="6">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="AR20" s="6">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
+      <c r="AR20" s="6">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
       <c r="AS20" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT20" s="19">
@@ -7027,8 +7098,12 @@
       <c r="AI21" s="7">
         <v>879.01604755108178</v>
       </c>
+      <c r="AJ21" s="7">
+        <f t="shared" si="7"/>
+        <v>0.91807197632885451</v>
+      </c>
       <c r="AK21" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL21" s="7">
@@ -7048,19 +7123,19 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="AP21" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ21" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AR21" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AS21" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT21" s="19">
@@ -7194,8 +7269,12 @@
       <c r="AI22" s="7">
         <v>924.89015080378601</v>
       </c>
+      <c r="AJ22" s="7">
+        <f t="shared" si="7"/>
+        <v>0.86713000382046779</v>
+      </c>
       <c r="AK22" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="AL22" s="7">
@@ -7215,19 +7294,19 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="AP22" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ22" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AR22" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS22" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="AT22" s="19">
@@ -7369,8 +7448,12 @@
       <c r="AI23" s="7">
         <v>924.89015080378601</v>
       </c>
+      <c r="AJ23" s="7">
+        <f t="shared" si="7"/>
+        <v>1.0714785957432464</v>
+      </c>
       <c r="AK23" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AL23" s="7">
@@ -7390,19 +7473,19 @@
         <v>0.5</v>
       </c>
       <c r="AP23" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ23" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AR23" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AS23" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT23" s="19">
@@ -7533,8 +7616,12 @@
       <c r="AI24" s="7">
         <v>898.37546314912686</v>
       </c>
+      <c r="AJ24" s="7">
+        <f t="shared" si="7"/>
+        <v>0.98177213890979942</v>
+      </c>
       <c r="AK24" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="AL24" s="7">
@@ -7554,19 +7641,19 @@
         <v>0.27272727272727271</v>
       </c>
       <c r="AP24" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ24" s="6">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="AR24" s="6">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
+      <c r="AR24" s="6">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
       <c r="AS24" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT24" s="19">
@@ -7712,8 +7799,12 @@
       <c r="AI25" s="7">
         <v>898.37546314912686</v>
       </c>
+      <c r="AJ25" s="7">
+        <f t="shared" si="7"/>
+        <v>1.0006951846710994</v>
+      </c>
       <c r="AK25" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="AL25" s="7">
@@ -7733,19 +7824,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AP25" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ25" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AR25" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="AS25" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT25" s="19">
@@ -7886,8 +7977,12 @@
       <c r="AI26" s="7">
         <v>898.37546314912686</v>
       </c>
+      <c r="AJ26" s="7">
+        <f t="shared" si="7"/>
+        <v>1.1910387626229992</v>
+      </c>
       <c r="AK26" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL26" s="7">
@@ -7907,19 +8002,19 @@
         <v>0.42857142857142855</v>
       </c>
       <c r="AP26" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ26" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AR26" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS26" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT26" s="19">
@@ -8055,8 +8150,12 @@
       <c r="AI27" s="7">
         <v>1052.9013865401105</v>
       </c>
+      <c r="AJ27" s="7">
+        <f t="shared" si="7"/>
+        <v>0.87947457552780406</v>
+      </c>
       <c r="AK27" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="AL27" s="7">
@@ -8076,19 +8175,19 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="AP27" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ27" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="AR27" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="AS27" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AT27" s="6">
@@ -8229,46 +8328,50 @@
         <v>0.26125244618395305</v>
       </c>
       <c r="AH28" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1022</v>
       </c>
       <c r="AI28" s="7">
         <v>1112.0405986835431</v>
       </c>
+      <c r="AJ28" s="7">
+        <f t="shared" si="7"/>
+        <v>0.91903119473323636</v>
+      </c>
       <c r="AK28" s="7">
-        <f t="shared" ref="AK28:AK33" si="13">SUM(AP28:AS28)</f>
+        <f t="shared" ref="AK28:AK33" si="14">SUM(AP28:AS28)</f>
         <v>9</v>
       </c>
       <c r="AL28" s="7">
-        <f t="shared" ref="AL28:AL33" si="14">AP28/$AK28</f>
+        <f t="shared" ref="AL28:AL33" si="15">AP28/$AK28</f>
         <v>0</v>
       </c>
       <c r="AM28" s="7">
-        <f t="shared" ref="AM28:AM33" si="15">AQ28/$AK28</f>
+        <f t="shared" ref="AM28:AM33" si="16">AQ28/$AK28</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AN28" s="7">
-        <f t="shared" ref="AN28:AN33" si="16">AR28/$AK28</f>
+        <f t="shared" ref="AN28:AN33" si="17">AR28/$AK28</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AO28" s="7">
-        <f t="shared" ref="AO28:AO33" si="17">AS28/$AK28</f>
+        <f t="shared" ref="AO28:AO33" si="18">AS28/$AK28</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AP28" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ28" s="6">
-        <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="AR28" s="6">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
+      <c r="AR28" s="6">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
       <c r="AS28" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT28" s="6">
@@ -8408,40 +8511,44 @@
       <c r="AI29" s="7">
         <v>1228.4313354492187</v>
       </c>
+      <c r="AJ29" s="7">
+        <f t="shared" si="7"/>
+        <v>0.95243418678517244</v>
+      </c>
       <c r="AK29" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="AL29" s="7">
-        <f t="shared" si="14"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="AM29" s="7">
         <f t="shared" si="15"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="AN29" s="7">
+      <c r="AM29" s="7">
         <f t="shared" si="16"/>
         <v>0.16666666666666666</v>
       </c>
+      <c r="AN29" s="7">
+        <f t="shared" si="17"/>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="AO29" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
       <c r="AP29" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AQ29" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AR29" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AS29" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT29" s="6">
@@ -8572,40 +8679,44 @@
       <c r="AI30" s="7">
         <v>1228.4313354492187</v>
       </c>
+      <c r="AJ30" s="7">
+        <f t="shared" si="7"/>
+        <v>0.81404631349160039</v>
+      </c>
       <c r="AK30" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="AL30" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AM30" s="7">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
+      <c r="AM30" s="7">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
       <c r="AN30" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="AO30" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="AP30" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AQ30" s="6">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AQ30" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="AR30" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="AS30" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="AT30" s="6">
@@ -8736,40 +8847,44 @@
       <c r="AI31" s="7">
         <v>1152.7054517341383</v>
       </c>
+      <c r="AJ31" s="7">
+        <f t="shared" si="7"/>
+        <v>0.91957576708371469</v>
+      </c>
       <c r="AK31" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="AL31" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AM31" s="7">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
+      <c r="AM31" s="7">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
       <c r="AN31" s="7">
-        <f t="shared" si="16"/>
-        <v>0.5</v>
-      </c>
-      <c r="AO31" s="7">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
+      <c r="AO31" s="7">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
       <c r="AP31" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AQ31" s="6">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AQ31" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="AR31" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AS31" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AT31" s="6">
@@ -8900,40 +9015,44 @@
       <c r="AI32" s="7">
         <v>1171.997577089252</v>
       </c>
+      <c r="AJ32" s="7">
+        <f t="shared" si="7"/>
+        <v>0.91638414702815629</v>
+      </c>
       <c r="AK32" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="AL32" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AM32" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.4</v>
       </c>
       <c r="AN32" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="AO32" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.1</v>
       </c>
       <c r="AP32" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ32" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="AR32" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="AS32" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="AT32" s="6">
@@ -9076,40 +9195,44 @@
       <c r="AI33" s="7">
         <v>886.96173502604165</v>
       </c>
+      <c r="AJ33" s="7">
+        <f t="shared" si="7"/>
+        <v>0.97636681020356964</v>
+      </c>
       <c r="AK33" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="AL33" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AM33" s="7">
-        <f t="shared" si="15"/>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="AN33" s="7">
         <f t="shared" si="16"/>
         <v>0.22222222222222221</v>
       </c>
+      <c r="AN33" s="7">
+        <f t="shared" si="17"/>
+        <v>0.22222222222222221</v>
+      </c>
       <c r="AO33" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="AP33" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AQ33" s="6">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="AR33" s="6">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
+      <c r="AR33" s="6">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
       <c r="AS33" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="AT33" s="6">
@@ -9462,77 +9585,77 @@
     </row>
     <row r="65" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J65" s="7">
-        <f t="shared" ref="J65:J113" si="18">BIN2DEC(CONCATENATE(H65,I65))+1</f>
+        <f t="shared" ref="J65:J113" si="19">BIN2DEC(CONCATENATE(H65,I65))+1</f>
         <v>1</v>
       </c>
       <c r="AD65" s="13"/>
     </row>
     <row r="66" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J66" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD66" s="13"/>
     </row>
     <row r="67" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J67" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD67" s="13"/>
     </row>
     <row r="68" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J68" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD68" s="13"/>
     </row>
     <row r="69" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J69" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD69" s="13"/>
     </row>
     <row r="70" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J70" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD70" s="13"/>
     </row>
     <row r="71" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J71" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD71" s="13"/>
     </row>
     <row r="72" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J72" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD72" s="13"/>
     </row>
     <row r="73" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J73" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD73" s="13"/>
     </row>
     <row r="74" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J74" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD74" s="13"/>
     </row>
     <row r="75" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J75" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD75" s="13"/>
@@ -9550,35 +9673,35 @@
     </row>
     <row r="76" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J76" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD76" s="13"/>
     </row>
     <row r="77" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J77" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD77" s="13"/>
     </row>
     <row r="78" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J78" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD78" s="13"/>
     </row>
     <row r="79" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J79" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD79" s="13"/>
     </row>
     <row r="80" spans="10:56" x14ac:dyDescent="0.25">
       <c r="J80" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="Q80" s="12"/>
@@ -9611,42 +9734,42 @@
     </row>
     <row r="81" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J81" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD81" s="13"/>
     </row>
     <row r="82" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J82" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD82" s="13"/>
     </row>
     <row r="83" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J83" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD83" s="13"/>
     </row>
     <row r="84" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J84" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD84" s="13"/>
     </row>
     <row r="85" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J85" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD85" s="13"/>
     </row>
     <row r="86" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J86" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD86" s="13"/>
@@ -9663,7 +9786,7 @@
     </row>
     <row r="87" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J87" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD87" s="13"/>
@@ -9679,14 +9802,14 @@
     </row>
     <row r="88" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J88" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD88" s="13"/>
     </row>
     <row r="89" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J89" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="Q89" s="12"/>
@@ -9712,7 +9835,7 @@
     </row>
     <row r="90" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J90" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD90" s="13"/>
@@ -9725,7 +9848,7 @@
     </row>
     <row r="91" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J91" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD91" s="13"/>
@@ -9742,14 +9865,14 @@
     </row>
     <row r="92" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J92" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD92" s="13"/>
     </row>
     <row r="93" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J93" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD93" s="13"/>
@@ -9773,28 +9896,28 @@
     </row>
     <row r="94" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J94" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD94" s="13"/>
     </row>
     <row r="95" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J95" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD95" s="13"/>
     </row>
     <row r="96" spans="10:62" x14ac:dyDescent="0.25">
       <c r="J96" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD96" s="13"/>
     </row>
     <row r="97" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J97" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="Q97" s="12"/>
@@ -9820,101 +9943,101 @@
     </row>
     <row r="98" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J98" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD98" s="13"/>
     </row>
     <row r="99" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J99" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD99" s="13"/>
     </row>
     <row r="100" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J100" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD100" s="13"/>
     </row>
     <row r="101" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J101" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AD101" s="13"/>
     </row>
     <row r="102" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J102" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J103" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J104" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J105" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J106" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J107" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J108" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J109" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J110" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J111" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="10:51" x14ac:dyDescent="0.25">
       <c r="J112" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J113" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -9961,7 +10084,7 @@
     </row>
     <row r="117" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J117" s="7">
-        <f t="shared" ref="J117:J143" si="19">BIN2DEC(CONCATENATE(H117,I117))+1</f>
+        <f t="shared" ref="J117:J143" si="20">BIN2DEC(CONCATENATE(H117,I117))+1</f>
         <v>1</v>
       </c>
     </row>
@@ -9972,7 +10095,7 @@
       <c r="H118" s="8"/>
       <c r="I118" s="8"/>
       <c r="J118" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="N118" s="7"/>
@@ -10014,7 +10137,7 @@
     </row>
     <row r="119" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J119" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q119" s="12"/>
@@ -10047,7 +10170,7 @@
     </row>
     <row r="120" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J120" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q120" s="12"/>
@@ -10082,7 +10205,7 @@
     </row>
     <row r="121" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J121" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q121" s="12"/>
@@ -10117,7 +10240,7 @@
     </row>
     <row r="122" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J122" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q122" s="12"/>
@@ -10149,7 +10272,7 @@
     </row>
     <row r="123" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J123" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q123" s="12"/>
@@ -10181,7 +10304,7 @@
     </row>
     <row r="124" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J124" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q124" s="12"/>
@@ -10218,7 +10341,7 @@
       <c r="H125" s="8"/>
       <c r="I125" s="8"/>
       <c r="J125" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="N125" s="7"/>
@@ -10276,7 +10399,7 @@
     </row>
     <row r="126" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J126" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q126" s="12"/>
@@ -10311,7 +10434,7 @@
     </row>
     <row r="127" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J127" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q127" s="12"/>
@@ -10343,7 +10466,7 @@
     </row>
     <row r="128" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J128" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q128" s="12"/>
@@ -10379,7 +10502,7 @@
     </row>
     <row r="129" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J129" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q129" s="12"/>
@@ -10413,7 +10536,7 @@
     </row>
     <row r="130" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J130" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q130" s="12"/>
@@ -10446,7 +10569,7 @@
     </row>
     <row r="131" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J131" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q131" s="12"/>
@@ -10485,7 +10608,7 @@
     </row>
     <row r="132" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J132" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q132" s="12"/>
@@ -10527,7 +10650,7 @@
       <c r="H133" s="8"/>
       <c r="I133" s="8"/>
       <c r="J133" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="N133" s="7"/>
@@ -10585,7 +10708,7 @@
     </row>
     <row r="134" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J134" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q134" s="12"/>
@@ -10617,7 +10740,7 @@
     </row>
     <row r="135" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J135" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q135" s="12"/>
@@ -10651,7 +10774,7 @@
     </row>
     <row r="136" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J136" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q136" s="12"/>
@@ -10684,7 +10807,7 @@
     </row>
     <row r="137" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J137" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q137" s="12"/>
@@ -10717,7 +10840,7 @@
     </row>
     <row r="138" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J138" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q138" s="12"/>
@@ -10755,7 +10878,7 @@
     </row>
     <row r="139" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J139" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q139" s="12"/>
@@ -10789,7 +10912,7 @@
     </row>
     <row r="140" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J140" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q140" s="12"/>
@@ -10824,7 +10947,7 @@
     </row>
     <row r="141" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J141" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q141" s="12"/>
@@ -10854,7 +10977,7 @@
     </row>
     <row r="142" spans="5:65" x14ac:dyDescent="0.25">
       <c r="J142" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="Q142" s="12"/>
@@ -10892,7 +11015,7 @@
       <c r="H143" s="8"/>
       <c r="I143" s="8"/>
       <c r="J143" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="N143" s="7"/>

</xml_diff>